<commit_message>
added new times to timesheet
</commit_message>
<xml_diff>
--- a/man/Project_Plan/TimeSheet.xlsx
+++ b/man/Project_Plan/TimeSheet.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="80">
   <si>
     <t>moniter and revew git submishions</t>
   </si>
@@ -267,6 +267,15 @@
   </si>
   <si>
     <t>create timsheet</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>card</t>
+  </si>
+  <si>
+    <t>web php</t>
   </si>
 </sst>
 </file>
@@ -305,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +331,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -372,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -384,14 +399,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -403,6 +412,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,19 +564,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A10:C22" totalsRowShown="0">
-  <autoFilter ref="A10:C22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A10:D22" totalsRowShown="0">
+  <autoFilter ref="A10:D22"/>
   <sortState ref="A11:C22">
     <sortCondition ref="A10:A22"/>
   </sortState>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="1" name="Member" dataDxfId="14"/>
-    <tableColumn id="2" name="Time Spent" dataDxfId="12">
+    <tableColumn id="2" name="Time Spent" dataDxfId="13">
       <calculatedColumnFormula>'Cormac Brady'!$J$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Hours left" dataDxfId="13">
+    <tableColumn id="3" name="Hours left" dataDxfId="12">
       <calculatedColumnFormula>$H$7-Table2[[#This Row],[Time Spent]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="4" name="card"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1036,7 +1053,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,142 +1066,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="8"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>41918</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>41999</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>42016</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>42051</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="12"/>
+      <c r="H4" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="5">
+      <c r="D5" s="13">
         <f>INT((E3-D3)/7)</f>
         <v>11</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13">
         <f>INT((G3-F3)/7)</f>
         <v>5</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6">
+      <c r="G5" s="13"/>
+      <c r="H5" s="5">
         <f>(D5+F5)</f>
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="12" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="5">
+      <c r="D7" s="13">
         <v>40</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13">
         <v>40</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="12">
+      <c r="G7" s="13"/>
+      <c r="H7" s="10">
         <f>D7+F7</f>
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="12" t="s">
+      <c r="G8" s="12"/>
+      <c r="H8" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="5">
+      <c r="D9" s="13">
         <f>INT(D7/D5)</f>
         <v>3</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
         <f>INT(F7/F5)</f>
         <v>8</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6">
+      <c r="G9" s="13"/>
+      <c r="H9" s="5">
         <f>D9+F9</f>
         <v>11</v>
       </c>
@@ -1199,6 +1216,9 @@
       <c r="C10" t="s">
         <v>44</v>
       </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1212,6 +1232,7 @@
         <f>$H$7-Table2[[#This Row],[Time Spent]]</f>
         <v>79</v>
       </c>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1232,11 +1253,11 @@
       </c>
       <c r="B13">
         <f>'Calvin Chan'!$J$6</f>
-        <v>4</v>
+        <v>6.75</v>
       </c>
       <c r="C13">
         <f>$H$7-Table2[[#This Row],[Time Spent]]</f>
-        <v>76</v>
+        <v>73.25</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1245,11 +1266,11 @@
       </c>
       <c r="B14">
         <f>'Cormac Brady'!$J$6</f>
-        <v>37.75</v>
+        <v>40.75</v>
       </c>
       <c r="C14">
         <f>$H$7-Table2[[#This Row],[Time Spent]]</f>
-        <v>42.25</v>
+        <v>39.25</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1258,11 +1279,11 @@
       </c>
       <c r="B15">
         <f>'Henry Hollingsworth'!$J$6</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <f>$H$7-Table2[[#This Row],[Time Spent]]</f>
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1278,7 +1299,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1291,7 +1312,7 @@
         <v>78.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -1304,7 +1325,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1316,8 +1337,9 @@
         <f>$H$7-Table2[[#This Row],[Time Spent]]</f>
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1330,7 +1352,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1343,21 +1365,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B22">
         <f>'Zach Yewman'!$J$6</f>
-        <v>4.5</v>
+        <v>13</v>
       </c>
       <c r="C22">
         <f>$H$7-Table2[[#This Row],[Time Spent]]</f>
-        <v>75.5</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="UKzY/ENi2O9Et9jDsA+QBu531hYk2IoD47GxHYmmNJNHHVYx0HWZf79aD+TdbUOYcF0bVxecHo6Dp22158608Q==" saltValue="wh2897ERhOP08ju7zBn5tw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
@@ -1447,10 +1468,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1475,35 +1496,35 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table111[Actual Time2])</f>
         <v>3</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table111[Actual Time])</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
         <v>3</v>
       </c>
@@ -1562,10 +1583,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1599,17 +1620,17 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table11113[Actual Time2])</f>
         <v>3</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table11113[Actual Time])</f>
         <v>0.25</v>
       </c>
@@ -1624,19 +1645,19 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
         <v>7</v>
       </c>
@@ -1695,10 +1716,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1723,17 +1744,17 @@
       <c r="F3">
         <v>5</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table1111314[Actual Time2])</f>
         <v>6</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table1111314[Actual Time])</f>
         <v>0</v>
       </c>
@@ -1745,19 +1766,19 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
         <v>6</v>
       </c>
@@ -1780,7 +1801,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,10 +1837,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1842,39 +1863,48 @@
         <v>10</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table111131415[Actual Time2])</f>
-        <v>4.5</v>
-      </c>
-      <c r="L3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table111131415[Actual Time])</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L4" s="6" t="s">
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
-        <v>4.5</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1892,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H11" sqref="H11:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,10 +1961,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1977,17 +2007,17 @@
       <c r="F3">
         <v>1.5</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table1[Actual Time2])</f>
-        <v>13.75</v>
-      </c>
-      <c r="L3" s="6" t="s">
+        <v>16.75</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table1[Actual Time])</f>
         <v>1.5</v>
       </c>
@@ -2002,10 +2032,10 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>24</v>
       </c>
@@ -2031,12 +2061,12 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
-        <v>37.75</v>
+        <v>40.75</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2070,6 +2100,17 @@
       </c>
       <c r="F9">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2126,10 +2167,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2145,36 +2186,36 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table15[Actual Time2])</f>
         <v>1</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="8"/>
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table15[Actual Time])</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
         <v>1</v>
       </c>
@@ -2233,10 +2274,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2261,17 +2302,17 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table16[Actual Time2])</f>
         <v>11</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table16[Actual Time])</f>
         <v>0</v>
       </c>
@@ -2286,10 +2327,10 @@
       <c r="F4">
         <v>3</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>0</v>
       </c>
@@ -2306,10 +2347,10 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
         <v>11</v>
       </c>
@@ -2332,7 +2373,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D2" sqref="D2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,10 +2409,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2382,6 +2423,9 @@
       <c r="E2">
         <v>0.5</v>
       </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
@@ -2393,17 +2437,17 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table17[Actual Time2])</f>
-        <v>4</v>
-      </c>
-      <c r="L3" s="6" t="s">
+        <v>6.75</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table17[Actual Time])</f>
         <v>0</v>
       </c>
@@ -2418,21 +2462,32 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.75</v>
+      </c>
+    </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
-        <v>4</v>
+        <v>6.75</v>
       </c>
     </row>
   </sheetData>
@@ -2453,7 +2508,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,10 +2544,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2517,17 +2572,17 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table18[Actual Time2])</f>
-        <v>8</v>
-      </c>
-      <c r="L3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table18[Actual Time])</f>
         <v>0</v>
       </c>
@@ -2540,12 +2595,12 @@
         <v>10</v>
       </c>
       <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="L4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>0</v>
       </c>
@@ -2562,12 +2617,12 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2624,10 +2679,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2652,35 +2707,35 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table1812[Actual Time2])</f>
         <v>2</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table1812[Actual Time])</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
         <v>10</v>
       </c>
@@ -2739,10 +2794,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2767,35 +2822,35 @@
       <c r="F3">
         <v>0.5</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table19[Actual Time2])</f>
         <v>1.5</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table19[Actual Time])</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
         <v>1.5</v>
       </c>
@@ -2854,10 +2909,10 @@
       <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2882,17 +2937,17 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>SUM(Table110[Actual Time2])</f>
         <v>5.5</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f>SUM(Table110[Actual Time])</f>
         <v>0</v>
       </c>
@@ -2907,19 +2962,19 @@
       <c r="F4">
         <v>0.5</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f>M3*Task_Table!H5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>SUM(J3,M4)</f>
         <v>5.5</v>
       </c>

</xml_diff>

<commit_message>
revert to aproved vershion
</commit_message>
<xml_diff>
--- a/man/Project_Plan/TimeSheet.xlsx
+++ b/man/Project_Plan/TimeSheet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cormac\Documents\GitHub\cs-221-group-project\man\Project_Plan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
   </bookViews>
   <sheets>
     <sheet name="Task_Table" sheetId="1" r:id="rId1"/>
@@ -21,12 +26,7 @@
     <sheet name="Scott Lockett" sheetId="12" r:id="rId12"/>
     <sheet name="Zach Yewman" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -907,24 +907,24 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="9" fillId="7" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="21" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -932,7 +932,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2257,20 +2257,20 @@
   <dimension ref="A1:IV23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1" customWidth="1"/>
     <col min="4" max="7" width="8" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="1" customWidth="1"/>
-    <col min="9" max="256" width="6.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.59765625" style="1" customWidth="1"/>
+    <col min="9" max="256" width="6.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" customHeight="1">
+    <row r="1" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2278,17 +2278,17 @@
         <v>1</v>
       </c>
       <c r="C1" s="4"/>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="57" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="58"/>
+      <c r="G1" s="56"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="17" customHeight="1">
+    <row r="2" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="17" customHeight="1">
+    <row r="3" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2332,110 +2332,110 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="17" customHeight="1">
+    <row r="4" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="57" t="s">
+      <c r="E4" s="56"/>
+      <c r="F4" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="58"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17" customHeight="1">
+    <row r="5" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="59">
+      <c r="D5" s="53">
         <f>INT((E3-D3)/7)</f>
         <v>11</v>
       </c>
-      <c r="E5" s="60"/>
-      <c r="F5" s="59">
+      <c r="E5" s="54"/>
+      <c r="F5" s="53">
         <f>INT((G3-F3)/7)</f>
         <v>5</v>
       </c>
-      <c r="G5" s="60"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="6">
         <f>(D5+F5)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17" customHeight="1">
+    <row r="6" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="57" t="s">
+      <c r="E6" s="56"/>
+      <c r="F6" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="58"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" customHeight="1">
+    <row r="7" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="59">
+      <c r="D7" s="53">
         <v>40</v>
       </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="59">
+      <c r="E7" s="54"/>
+      <c r="F7" s="53">
         <v>40</v>
       </c>
-      <c r="G7" s="60"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="2">
         <f>D7+F7</f>
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" customHeight="1">
+    <row r="8" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="57" t="s">
+      <c r="E8" s="56"/>
+      <c r="F8" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="58"/>
+      <c r="G8" s="56"/>
       <c r="H8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" customHeight="1">
+    <row r="9" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="59">
+      <c r="D9" s="53">
         <f>INT(D7/D5)</f>
         <v>3</v>
       </c>
-      <c r="E9" s="60"/>
-      <c r="F9" s="59">
+      <c r="E9" s="54"/>
+      <c r="F9" s="53">
         <f>INT(F7/F5)</f>
         <v>8</v>
       </c>
-      <c r="G9" s="60"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="6">
         <f>D9+F9</f>
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" customHeight="1">
+    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2453,7 +2453,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1">
+    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
@@ -2471,7 +2471,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" customHeight="1">
+    <row r="12" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>19</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1">
+    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>20</v>
       </c>
@@ -2507,7 +2507,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="16.5" customHeight="1">
+    <row r="14" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>21</v>
       </c>
@@ -2525,7 +2525,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" ht="16.5" customHeight="1">
+    <row r="15" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>22</v>
       </c>
@@ -2543,16 +2543,17 @@
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:8" ht="16.5" customHeight="1">
+    <row r="16" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="26">
-        <v>21</v>
+        <f>'Rhys Howard'!$J$6</f>
+        <v>10</v>
       </c>
       <c r="C16" s="27">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="24"/>
@@ -2560,7 +2561,7 @@
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" ht="16.5" customHeight="1">
+    <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>24</v>
       </c>
@@ -2578,7 +2579,7 @@
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" ht="16.5" customHeight="1">
+    <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>25</v>
       </c>
@@ -2596,25 +2597,25 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A19" s="54" t="s">
+    <row r="19" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="55">
+      <c r="B19" s="59">
         <f>'Kieran Lynch'!$J$6</f>
         <v>3</v>
       </c>
-      <c r="C19" s="56">
+      <c r="C19" s="60">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="D19" s="53"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="24"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8" ht="16.5" customHeight="1">
+    <row r="20" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>27</v>
       </c>
@@ -2632,7 +2633,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" ht="16.5" customHeight="1">
+    <row r="21" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>28</v>
       </c>
@@ -2650,7 +2651,7 @@
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>29</v>
       </c>
@@ -2668,7 +2669,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:8" ht="17" customHeight="1">
+    <row r="23" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
@@ -2680,6 +2681,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="D6:E6"/>
@@ -2688,23 +2695,12 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2714,24 +2710,24 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="46" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="46" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="46" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="46" customWidth="1"/>
     <col min="4" max="4" width="23" style="46" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="46" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="46" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="46" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="46" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="46" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="46" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="46" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="46" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="46" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="46" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="46" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="46" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="46" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="46" customWidth="1"/>
     <col min="13" max="13" width="8" style="46" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="46" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -2762,7 +2758,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -2783,7 +2779,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -2814,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -2834,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -2849,7 +2845,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -2869,7 +2865,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -2884,7 +2880,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -2899,7 +2895,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -2914,7 +2910,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -2929,7 +2925,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -2944,7 +2940,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -2959,7 +2955,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -2974,7 +2970,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -2989,7 +2985,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -3004,7 +3000,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -3019,7 +3015,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -3034,7 +3030,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -3049,7 +3045,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -3064,7 +3060,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -3079,7 +3075,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -3094,7 +3090,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -3109,7 +3105,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -3124,7 +3120,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -3139,7 +3135,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -3154,7 +3150,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -3169,7 +3165,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -3184,7 +3180,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -3199,7 +3195,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -3220,11 +3216,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3236,24 +3227,24 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="47" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="47" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="47" customWidth="1"/>
-    <col min="4" max="4" width="18.375" style="47" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="47" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="47" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="47" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="47" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="47" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="47" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="47" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="47" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="47" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="47" customWidth="1"/>
+    <col min="4" max="4" width="18.3984375" style="47" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="47" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="47" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="47" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="47" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="47" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="47" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="47" customWidth="1"/>
     <col min="13" max="13" width="8" style="47" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="47" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -3284,7 +3275,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>75</v>
       </c>
@@ -3311,7 +3302,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -3342,7 +3333,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -3368,7 +3359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -3389,7 +3380,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -3415,7 +3406,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -3430,7 +3421,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -3445,7 +3436,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -3460,7 +3451,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -3475,7 +3466,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -3490,7 +3481,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -3505,7 +3496,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -3520,7 +3511,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -3535,7 +3526,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -3550,7 +3541,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -3565,7 +3556,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -3580,7 +3571,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -3595,7 +3586,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -3610,7 +3601,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -3625,7 +3616,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -3640,7 +3631,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -3655,7 +3646,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -3670,7 +3661,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -3685,7 +3676,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -3700,7 +3691,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -3715,7 +3706,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -3730,7 +3721,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -3745,7 +3736,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -3766,11 +3757,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3782,24 +3768,24 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="48" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="48" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="48" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="48" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="48" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="48" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="48" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="48" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="48" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="48" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="48" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="48" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="48" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="48" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="48" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="48" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="48" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="48" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="48" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="48" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="48" customWidth="1"/>
     <col min="13" max="13" width="8" style="48" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="48" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -3830,7 +3816,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -3851,7 +3837,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -3882,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -3908,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -3929,7 +3915,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -3949,7 +3935,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -3964,7 +3950,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -3979,7 +3965,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -3994,7 +3980,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -4009,7 +3995,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -4024,7 +4010,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -4039,7 +4025,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -4054,7 +4040,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -4069,7 +4055,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -4084,7 +4070,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -4099,7 +4085,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -4114,7 +4100,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -4129,7 +4115,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -4144,7 +4130,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -4159,7 +4145,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -4174,7 +4160,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -4189,7 +4175,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -4204,7 +4190,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -4219,7 +4205,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -4234,7 +4220,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -4249,7 +4235,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -4264,7 +4250,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -4279,7 +4265,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -4300,11 +4286,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4316,24 +4297,24 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="49" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="19.75" style="49" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="49" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="49" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="49" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="49" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="49" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="49" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="49" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="19.69921875" style="49" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="49" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="49" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="49" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="49" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="49" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="49" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="49" customWidth="1"/>
     <col min="13" max="13" width="8" style="49" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="49" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -4364,7 +4345,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -4385,7 +4366,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -4416,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -4442,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -4457,7 +4438,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -4477,7 +4458,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -4492,7 +4473,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -4507,7 +4488,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -4522,7 +4503,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -4537,7 +4518,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -4552,7 +4533,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -4567,7 +4548,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -4582,7 +4563,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -4597,7 +4578,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -4612,7 +4593,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -4627,7 +4608,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -4642,7 +4623,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -4657,7 +4638,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -4672,7 +4653,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -4687,7 +4668,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -4702,7 +4683,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -4717,7 +4698,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -4732,7 +4713,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -4747,7 +4728,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -4762,7 +4743,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -4777,7 +4758,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -4792,7 +4773,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -4807,7 +4788,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -4828,11 +4809,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4844,24 +4820,24 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="32" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="32" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="24.625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="32" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="32" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="32" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="32" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="32" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="32" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="32" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="32" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="32" customWidth="1"/>
+    <col min="4" max="4" width="24.59765625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="32" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="32" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="32" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="32" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="32" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="32" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="32" customWidth="1"/>
     <col min="13" max="13" width="8" style="32" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="32" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -4892,7 +4868,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>37</v>
       </c>
@@ -4919,7 +4895,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
@@ -4956,7 +4932,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -4982,7 +4958,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -5003,7 +4979,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -5029,7 +5005,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -5050,7 +5026,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -5071,7 +5047,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -5092,7 +5068,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -5113,7 +5089,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -5128,7 +5104,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -5143,7 +5119,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -5158,7 +5134,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -5173,7 +5149,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -5188,7 +5164,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -5203,7 +5179,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -5218,7 +5194,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -5233,7 +5209,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -5248,7 +5224,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -5263,7 +5239,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -5278,7 +5254,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -5293,7 +5269,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -5308,7 +5284,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -5323,7 +5299,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -5338,7 +5314,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -5353,7 +5329,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -5368,7 +5344,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -5383,7 +5359,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -5404,11 +5380,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5420,24 +5391,24 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="38" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="38" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="38" customWidth="1"/>
-    <col min="4" max="4" width="18.375" style="38" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="38" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="38" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="38" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="38" customWidth="1"/>
-    <col min="10" max="10" width="15.375" style="38" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="38" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="38" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="38" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="38" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="18.3984375" style="38" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="38" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="38" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="38" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="38" customWidth="1"/>
+    <col min="10" max="10" width="15.3984375" style="38" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="38" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="38" customWidth="1"/>
     <col min="13" max="13" width="8" style="38" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="38" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -5468,7 +5439,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -5489,7 +5460,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -5520,7 +5491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -5540,7 +5511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -5555,7 +5526,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -5575,7 +5546,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -5590,7 +5561,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -5605,7 +5576,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -5620,7 +5591,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -5635,7 +5606,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -5650,7 +5621,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -5665,7 +5636,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -5680,7 +5651,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -5695,7 +5666,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -5710,7 +5681,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -5725,7 +5696,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -5740,7 +5711,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -5755,7 +5726,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -5770,7 +5741,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -5785,7 +5756,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -5800,7 +5771,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -5815,7 +5786,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -5830,7 +5801,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -5845,7 +5816,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -5860,7 +5831,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -5875,7 +5846,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -5890,7 +5861,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -5905,7 +5876,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -5922,15 +5893,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5942,24 +5908,24 @@
       <selection activeCell="D7" sqref="D7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="40" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="40" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="40" customWidth="1"/>
-    <col min="4" max="4" width="22.875" style="40" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="40" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="40" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="40" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="40" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="40" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="40" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="40" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="22.8984375" style="40" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="40" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="40" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="40" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="40" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="40" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="40" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="40" customWidth="1"/>
     <col min="13" max="13" width="8" style="40" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="40" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -5990,7 +5956,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -6011,7 +5977,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -6042,7 +6008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -6068,7 +6034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -6089,7 +6055,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -6115,7 +6081,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -6136,7 +6102,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -6151,7 +6117,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -6166,7 +6132,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -6181,7 +6147,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -6196,7 +6162,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -6211,7 +6177,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -6226,7 +6192,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -6241,7 +6207,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -6256,7 +6222,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -6271,7 +6237,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -6286,7 +6252,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -6301,7 +6267,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -6316,7 +6282,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -6331,7 +6297,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -6346,7 +6312,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -6361,7 +6327,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -6376,7 +6342,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -6391,7 +6357,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -6406,7 +6372,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -6421,7 +6387,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -6436,7 +6402,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -6451,7 +6417,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -6472,11 +6438,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6488,24 +6449,24 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="41" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="41" customWidth="1"/>
-    <col min="4" max="4" width="17.625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="41" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="41" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="41" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="41" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="41" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="41" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="41" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="41" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="41" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="41" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="41" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="41" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="41" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="41" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="41" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="41" customWidth="1"/>
     <col min="13" max="13" width="8" style="41" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="41" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -6536,7 +6497,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -6557,7 +6518,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -6588,7 +6549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -6614,7 +6575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -6635,7 +6596,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -6661,7 +6622,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -6676,7 +6637,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -6691,7 +6652,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -6706,7 +6667,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -6721,7 +6682,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -6736,7 +6697,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -6751,7 +6712,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -6766,7 +6727,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -6781,7 +6742,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -6796,7 +6757,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -6811,7 +6772,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -6826,7 +6787,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -6841,7 +6802,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -6856,7 +6817,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -6871,7 +6832,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -6886,7 +6847,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -6901,7 +6862,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -6916,7 +6877,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -6931,7 +6892,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -6946,7 +6907,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -6961,7 +6922,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -6976,7 +6937,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -6991,7 +6952,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -7012,11 +6973,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7028,23 +6984,23 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="42" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="42" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="42" customWidth="1"/>
-    <col min="4" max="4" width="18.375" style="42" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="42" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="42" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="42" customWidth="1"/>
-    <col min="9" max="10" width="14.625" style="42" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="42" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="42" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="42" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="42" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="42" customWidth="1"/>
+    <col min="4" max="4" width="18.3984375" style="42" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="42" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="42" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="42" customWidth="1"/>
+    <col min="9" max="10" width="14.59765625" style="42" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="42" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="42" customWidth="1"/>
     <col min="13" max="13" width="8" style="42" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="42" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -7075,7 +7031,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -7096,7 +7052,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -7127,7 +7083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -7153,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -7174,7 +7130,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -7200,7 +7156,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -7215,7 +7171,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -7230,7 +7186,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -7245,7 +7201,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -7260,7 +7216,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -7275,7 +7231,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -7290,7 +7246,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -7305,7 +7261,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -7320,7 +7276,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -7335,7 +7291,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -7350,7 +7306,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -7365,7 +7321,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -7380,7 +7336,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -7395,7 +7351,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -7410,7 +7366,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -7425,7 +7381,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -7440,7 +7396,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -7455,7 +7411,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -7470,7 +7426,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -7485,7 +7441,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -7500,7 +7456,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -7515,7 +7471,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -7530,7 +7486,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -7551,11 +7507,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7565,23 +7516,23 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="43" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="43" customWidth="1"/>
-    <col min="4" max="4" width="19.375" style="43" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="43" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="43" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="43" customWidth="1"/>
-    <col min="9" max="10" width="14.625" style="43" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="43" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="43" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="43" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="43" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="43" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" style="43" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="43" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="43" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="43" customWidth="1"/>
+    <col min="9" max="10" width="14.59765625" style="43" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="43" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="43" customWidth="1"/>
     <col min="13" max="13" width="8" style="43" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="43" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -7612,7 +7563,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>66</v>
       </c>
@@ -7639,7 +7590,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -7664,7 +7615,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -7684,7 +7635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -7699,7 +7650,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -7719,7 +7670,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -7734,7 +7685,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -7749,7 +7700,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -7764,7 +7715,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -7779,7 +7730,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -7794,7 +7745,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -7809,7 +7760,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -7824,7 +7775,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -7839,7 +7790,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -7854,7 +7805,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -7869,7 +7820,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -7884,7 +7835,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -7899,7 +7850,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -7914,7 +7865,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -7929,7 +7880,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -7944,7 +7895,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -7959,7 +7910,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -7974,7 +7925,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -7989,7 +7940,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -8004,7 +7955,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -8019,7 +7970,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -8034,7 +7985,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -8049,7 +8000,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -8070,11 +8021,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8086,24 +8032,24 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="44" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="44" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="44" customWidth="1"/>
-    <col min="4" max="4" width="21.375" style="44" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="44" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="44" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="44" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="44" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="44" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="44" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="44" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="44" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="44" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="44" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" style="44" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="44" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="44" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="44" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="44" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="44" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="44" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="44" customWidth="1"/>
     <col min="13" max="13" width="8" style="44" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="44" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -8134,7 +8080,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -8155,7 +8101,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -8186,7 +8132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -8212,7 +8158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -8233,7 +8179,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -8253,7 +8199,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -8268,7 +8214,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -8283,7 +8229,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -8298,7 +8244,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -8313,7 +8259,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -8328,7 +8274,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -8343,7 +8289,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -8358,7 +8304,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -8373,7 +8319,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -8388,7 +8334,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -8403,7 +8349,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -8418,7 +8364,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -8433,7 +8379,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -8448,7 +8394,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -8463,7 +8409,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -8478,7 +8424,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -8493,7 +8439,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -8508,7 +8454,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -8523,7 +8469,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -8538,7 +8484,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -8553,7 +8499,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -8568,7 +8514,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -8583,7 +8529,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -8604,11 +8550,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8620,24 +8561,24 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="45" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="45" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="45" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" style="45" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="45" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" style="45" customWidth="1"/>
     <col min="4" max="4" width="22" style="45" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="45" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="45" customWidth="1"/>
-    <col min="7" max="8" width="6.625" style="45" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="45" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="45" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="45" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="45" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" style="45" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="45" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="45" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" style="45" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="45" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="45" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" style="45" customWidth="1"/>
     <col min="13" max="13" width="8" style="45" customWidth="1"/>
-    <col min="14" max="256" width="6.625" style="45" customWidth="1"/>
+    <col min="14" max="256" width="6.59765625" style="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.5" customHeight="1">
+    <row r="1" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -8668,7 +8609,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="17.5" customHeight="1">
+    <row r="2" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -8689,7 +8630,7 @@
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -8720,7 +8661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1">
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -8746,7 +8687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" customHeight="1">
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -8767,7 +8708,7 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1">
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -8793,7 +8734,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -8808,7 +8749,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
@@ -8823,7 +8764,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -8838,7 +8779,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -8853,7 +8794,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="17" customHeight="1">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -8868,7 +8809,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="17" customHeight="1">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -8883,7 +8824,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="17" customHeight="1">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -8898,7 +8839,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="17" customHeight="1">
+    <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -8913,7 +8854,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="17" customHeight="1">
+    <row r="15" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -8928,7 +8869,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="17" customHeight="1">
+    <row r="16" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -8943,7 +8884,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="17" customHeight="1">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -8958,7 +8899,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="17" customHeight="1">
+    <row r="18" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -8973,7 +8914,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="17" customHeight="1">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -8988,7 +8929,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="17" customHeight="1">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -9003,7 +8944,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="17" customHeight="1">
+    <row r="21" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -9018,7 +8959,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="17" customHeight="1">
+    <row r="22" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -9033,7 +8974,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="17" customHeight="1">
+    <row r="23" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -9048,7 +8989,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="17" customHeight="1">
+    <row r="24" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -9063,7 +9004,7 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="17" customHeight="1">
+    <row r="25" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -9078,7 +9019,7 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="17" customHeight="1">
+    <row r="26" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -9093,7 +9034,7 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="17" customHeight="1">
+    <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -9108,7 +9049,7 @@
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" ht="17" customHeight="1">
+    <row r="28" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -9123,7 +9064,7 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" ht="17" customHeight="1">
+    <row r="29" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -9144,10 +9085,5 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>